<commit_message>
Modificada la descarga de facturas
</commit_message>
<xml_diff>
--- a/templates/report/facturas.xlsx
+++ b/templates/report/facturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\templates\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://manpowergroupapps-my.sharepoint.com/personal/cesar_ramos_ciberexperis_es/Documents/Documents/Cotown/git/cotown-back/templates/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732F741-D7F5-45BA-A904-60890E5C9A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{A732F741-D7F5-45BA-A904-60890E5C9A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77C0AD19-F2B4-4CDE-A812-A8A5828DC0E2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facturas" sheetId="41" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>.</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fecha de emision </t>
   </si>
   <si>
@@ -50,13 +47,64 @@
     <t>Importe</t>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
     <t>Issued_date</t>
   </si>
   <si>
-    <t>Concept</t>
+    <t>Bill_type</t>
+  </si>
+  <si>
+    <t>Tipo de factura</t>
+  </si>
+  <si>
+    <t>Codigo de factura</t>
+  </si>
+  <si>
+    <t>Bill_concept</t>
+  </si>
+  <si>
+    <t>Bill_code</t>
+  </si>
+  <si>
+    <t>Emitida</t>
+  </si>
+  <si>
+    <t>Issued</t>
+  </si>
+  <si>
+    <t>Método de pago</t>
+  </si>
+  <si>
+    <t>Payment_method</t>
+  </si>
+  <si>
+    <t>Nombre cliente</t>
+  </si>
+  <si>
+    <t>Customer_name</t>
+  </si>
+  <si>
+    <t>Nombre proveedor</t>
+  </si>
+  <si>
+    <t>Resource_provider_name</t>
+  </si>
+  <si>
+    <t>Código SAP</t>
+  </si>
+  <si>
+    <t>SAP_code</t>
+  </si>
+  <si>
+    <t>Tipo de recurso</t>
+  </si>
+  <si>
+    <t>Resource_type</t>
+  </si>
+  <si>
+    <t>Direccion del recurso</t>
+  </si>
+  <si>
+    <t>Resource_address</t>
   </si>
   <si>
     <t>Total</t>
@@ -66,10 +114,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -102,6 +151,17 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -145,12 +205,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -169,9 +230,16 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Moneda" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
@@ -556,54 +624,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48469C1-5DA9-43F7-A0B7-76DC91FAD532}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="7" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="33.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.42578125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5"/>
+      <c r="E3" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -612,6 +737,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001BDC921D6C313740BA67D7760DC75571" ma:contentTypeVersion="9" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ec6cd274e87ab0abf30bec2e834aaf15">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="220d4249-f262-4642-a86b-ff46de6e315d" xmlns:ns3="965e701d-44ad-4371-a199-8fefe953808c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e77808c4f084d99d477d3de919e85b9" ns2:_="" ns3:_="">
     <xsd:import namespace="220d4249-f262-4642-a86b-ff46de6e315d"/>
@@ -808,27 +953,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="220d4249-f262-4642-a86b-ff46de6e315d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
+    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2190EF49-E186-4D77-87E3-BC317999ED9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -845,23 +989,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC650EC1-3E41-4FC6-BA6C-52921951A8DA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="220d4249-f262-4642-a86b-ff46de6e315d"/>
-    <ds:schemaRef ds:uri="965e701d-44ad-4371-a199-8fefe953808c"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91323775-37AE-44DC-8259-7FCDE5D849E0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>